<commit_message>
poprawianie sposobu generacji rysunkow
</commit_message>
<xml_diff>
--- a/wyniki_BAT/srednie_bat_nowe_ drop_wave.bat .xlsx
+++ b/wyniki_BAT/srednie_bat_nowe_ drop_wave.bat .xlsx
@@ -145,25 +145,25 @@
         <v>20.0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.11949689391465926</v>
+        <v>-0.2503095220229778</v>
       </c>
       <c r="E2" t="n">
-        <v>0.14319074635780246</v>
+        <v>-0.1763863393679236</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.7639821600523498</v>
+        <v>-0.7965243440797991</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07378157789356349</v>
+        <v>0.0636078949626635</v>
       </c>
       <c r="H2" t="n">
-        <v>0.13581634177773508</v>
+        <v>0.15052815998841365</v>
       </c>
       <c r="I2" t="n">
-        <v>41.04</v>
+        <v>42.24</v>
       </c>
       <c r="J2" t="n">
-        <v>0.010799999999998136</v>
+        <v>0.010599999999999454</v>
       </c>
     </row>
     <row r="3">
@@ -177,25 +177,25 @@
         <v>40.0</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.010397900908621329</v>
+        <v>0.0446605239657579</v>
       </c>
       <c r="E3" t="n">
-        <v>0.04295855729038641</v>
+        <v>-0.0031689563581591175</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.8849472933108156</v>
+        <v>-0.8844470535815837</v>
       </c>
       <c r="G3" t="n">
-        <v>0.022304819834590116</v>
+        <v>0.020571135597453636</v>
       </c>
       <c r="H3" t="n">
-        <v>0.09619121325904757</v>
+        <v>0.08582523873282964</v>
       </c>
       <c r="I3" t="n">
-        <v>40.16</v>
+        <v>37.38</v>
       </c>
       <c r="J3" t="n">
-        <v>0.019200000000000158</v>
+        <v>0.014599999999999369</v>
       </c>
     </row>
     <row r="4">
@@ -209,25 +209,25 @@
         <v>70.0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.011531903237913359</v>
+        <v>-0.027543300257815494</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03541978389758252</v>
+        <v>0.005963237582247973</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.9277159291764564</v>
+        <v>-0.9177263510549409</v>
       </c>
       <c r="G4" t="n">
-        <v>0.008308612446978609</v>
+        <v>0.00975936843675343</v>
       </c>
       <c r="H4" t="n">
-        <v>0.05609417693373348</v>
+        <v>0.05523987695624826</v>
       </c>
       <c r="I4" t="n">
-        <v>39.0</v>
+        <v>35.88</v>
       </c>
       <c r="J4" t="n">
-        <v>0.03300000000000068</v>
+        <v>0.031399999999999866</v>
       </c>
     </row>
     <row r="5">
@@ -241,25 +241,25 @@
         <v>100.0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.038525843053442775</v>
+        <v>-0.0013303825928988084</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.020014002131429273</v>
+        <v>0.01252090016666907</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.9297658741340813</v>
+        <v>-0.93359115188267</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0064123418466251764</v>
+        <v>0.006168462354453858</v>
       </c>
       <c r="H5" t="n">
-        <v>0.038854902909118194</v>
+        <v>0.04235813352471028</v>
       </c>
       <c r="I5" t="n">
-        <v>34.58</v>
+        <v>31.66</v>
       </c>
       <c r="J5" t="n">
-        <v>0.05199999999999932</v>
+        <v>0.033800000000000094</v>
       </c>
     </row>
     <row r="6">
@@ -273,25 +273,25 @@
         <v>200.0</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.0640508233113636</v>
+        <v>-0.048219976174124865</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.04646955817595314</v>
+        <v>-0.0499739180099125</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.9400706036940706</v>
+        <v>-0.941345699488123</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0038207787336187586</v>
+        <v>0.003739485570970672</v>
       </c>
       <c r="H6" t="n">
-        <v>0.015294596619081603</v>
+        <v>0.017471802426589172</v>
       </c>
       <c r="I6" t="n">
-        <v>36.72</v>
+        <v>34.84</v>
       </c>
       <c r="J6" t="n">
-        <v>0.12839999999999974</v>
+        <v>0.12240000000000023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>